<commit_message>
Add initial test cases
</commit_message>
<xml_diff>
--- a/Unit 2/Project 1 Part 1/Test Cases.xlsx
+++ b/Unit 2/Project 1 Part 1/Test Cases.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurella/Desktop/CSE565TA/Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandoflores/Desktop/Fall 21/CSE565/Unit 2/Project 1 Part 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65219241-6487-664A-B383-B8971D1CFB7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ECA453-8D86-C540-AC61-C7EEE14B057A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10760" windowWidth="33600" windowHeight="10240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Matrix" sheetId="2" r:id="rId1"/>
     <sheet name="Defect Tracking " sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="42">
   <si>
     <t>Defect Description</t>
   </si>
@@ -89,13 +98,76 @@
   </si>
   <si>
     <t xml:space="preserve">Defect Number </t>
+  </si>
+  <si>
+    <t>Brando</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>BrandoBran</t>
+  </si>
+  <si>
+    <t>BrandoBrand</t>
+  </si>
+  <si>
+    <t>(empty)</t>
+  </si>
+  <si>
+    <t>Brand0</t>
+  </si>
+  <si>
+    <t>Bran_do</t>
+  </si>
+  <si>
+    <t>Bran-do</t>
+  </si>
+  <si>
+    <t>Bran$do</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>= Should fail</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>Sping</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>No discount given</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,6 +185,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -146,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,6 +247,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541407C-F33E-B246-BDA0-B1FB1801AAFA}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,6 +606,9 @@
         <v>10</v>
       </c>
       <c r="I3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -549,8 +637,14 @@
       <c r="H4" s="1">
         <v>5</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -562,87 +656,1800 @@
       <c r="A7" s="1">
         <v>1</v>
       </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
+      <c r="A16" s="1">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>100000000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>24</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <v>24</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37">
+        <v>24</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40">
+        <v>24</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42">
+        <v>24</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43">
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" t="s">
+        <v>34</v>
+      </c>
+      <c r="G43" t="s">
+        <v>36</v>
+      </c>
+      <c r="H43">
+        <v>5</v>
+      </c>
+      <c r="I43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44">
+        <v>24</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" t="s">
+        <v>32</v>
+      </c>
+      <c r="F44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45">
+        <v>24</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46">
+        <v>24</v>
+      </c>
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="I46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47">
+        <v>24</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47" t="s">
+        <v>36</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>43</v>
+      </c>
+      <c r="B49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49">
+        <v>24</v>
+      </c>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" t="s">
+        <v>37</v>
+      </c>
+      <c r="G49" t="s">
+        <v>36</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="I49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50">
+        <v>24</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" t="s">
+        <v>37</v>
+      </c>
+      <c r="G50" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51">
+        <v>24</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" t="s">
+        <v>36</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52">
+        <v>24</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="I52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>47</v>
+      </c>
+      <c r="B53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53">
+        <v>24</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
+      <c r="I53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>48</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54">
+        <v>24</v>
+      </c>
+      <c r="D54" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>49</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55">
+        <v>24</v>
+      </c>
+      <c r="D55" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G55" t="s">
+        <v>36</v>
+      </c>
+      <c r="H55">
+        <v>5</v>
+      </c>
+      <c r="I55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>50</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56">
+        <v>24</v>
+      </c>
+      <c r="D56" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56">
+        <v>5</v>
+      </c>
+      <c r="I56" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <v>51</v>
+      </c>
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57">
+        <v>24</v>
+      </c>
+      <c r="D57" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" t="s">
+        <v>37</v>
+      </c>
+      <c r="G57" t="s">
+        <v>36</v>
+      </c>
+      <c r="H57">
+        <v>5</v>
+      </c>
+      <c r="I57" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>52</v>
+      </c>
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58">
+        <v>24</v>
+      </c>
+      <c r="D58" t="s">
+        <v>30</v>
+      </c>
+      <c r="E58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" t="s">
+        <v>37</v>
+      </c>
+      <c r="G58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58">
+        <v>5</v>
+      </c>
+      <c r="I58" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
+        <v>53</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59">
+        <v>24</v>
+      </c>
+      <c r="D59" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" t="s">
+        <v>33</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H59">
+        <v>5</v>
+      </c>
+      <c r="I59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>54</v>
+      </c>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60">
+        <v>24</v>
+      </c>
+      <c r="D60" t="s">
+        <v>30</v>
+      </c>
+      <c r="E60" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="I60" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
+        <v>55</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61">
+        <v>24</v>
+      </c>
+      <c r="D61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H61">
+        <v>5</v>
+      </c>
+      <c r="I61" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>56</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62">
+        <v>24</v>
+      </c>
+      <c r="D62" t="s">
+        <v>30</v>
+      </c>
+      <c r="E62" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62">
+        <v>5</v>
+      </c>
+      <c r="I62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
+        <v>57</v>
+      </c>
+      <c r="B63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63">
+        <v>24</v>
+      </c>
+      <c r="D63" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H63">
+        <v>5</v>
+      </c>
+      <c r="I63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>58</v>
+      </c>
+      <c r="B64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64">
+        <v>24</v>
+      </c>
+      <c r="D64" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
+      </c>
+      <c r="I64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
+        <v>59</v>
+      </c>
+      <c r="B65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65">
+        <v>24</v>
+      </c>
+      <c r="D65" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H65">
+        <v>5</v>
+      </c>
+      <c r="I65" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>60</v>
+      </c>
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66">
+        <v>24</v>
+      </c>
+      <c r="D66" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="5">
+        <v>61</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" s="12">
+        <v>24</v>
+      </c>
+      <c r="D67" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" t="s">
+        <v>38</v>
+      </c>
+      <c r="G67" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>62</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" s="12">
+        <v>24</v>
+      </c>
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" t="s">
+        <v>38</v>
+      </c>
+      <c r="G68" t="s">
+        <v>17</v>
+      </c>
+      <c r="H68">
+        <v>10</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="9">
+        <v>63</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" s="12">
+        <v>24</v>
+      </c>
+      <c r="D69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" t="s">
+        <v>38</v>
+      </c>
+      <c r="G69" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69" s="2">
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="9">
+        <v>64</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" s="12">
+        <v>24</v>
+      </c>
+      <c r="D70" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" t="s">
+        <v>38</v>
+      </c>
+      <c r="G70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70" s="2">
+        <v>11</v>
+      </c>
+      <c r="I70" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="12"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add final set of test case results
</commit_message>
<xml_diff>
--- a/Unit 2/Project 1 Part 1/Test Cases.xlsx
+++ b/Unit 2/Project 1 Part 1/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandoflores/Desktop/Fall 21/CSE565/Unit 2/Project 1 Part 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ECA453-8D86-C540-AC61-C7EEE14B057A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261AC3EA-8BCF-4541-881B-938474D99530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10760" windowWidth="33600" windowHeight="10240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1760" windowWidth="33600" windowHeight="19240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Matrix" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="42">
   <si>
     <t>Defect Description</t>
   </si>
@@ -225,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +253,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541407C-F33E-B246-BDA0-B1FB1801AAFA}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,6 +1026,9 @@
       <c r="H19">
         <v>5</v>
       </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1051,6 +1055,9 @@
       <c r="H20">
         <v>5</v>
       </c>
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1076,6 +1083,9 @@
       </c>
       <c r="H21">
         <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1103,6 +1113,9 @@
       <c r="H22">
         <v>5</v>
       </c>
+      <c r="I22" s="13">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1128,6 +1141,9 @@
       </c>
       <c r="H23">
         <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1155,6 +1171,9 @@
       <c r="H24">
         <v>5</v>
       </c>
+      <c r="I24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1181,6 +1200,9 @@
       <c r="H25">
         <v>5</v>
       </c>
+      <c r="I25" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1207,6 +1229,9 @@
       <c r="H26">
         <v>5</v>
       </c>
+      <c r="I26" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1232,6 +1257,9 @@
       </c>
       <c r="H27">
         <v>5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1259,6 +1287,9 @@
       <c r="H28">
         <v>5</v>
       </c>
+      <c r="I28" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
@@ -1285,6 +1316,9 @@
       <c r="H29">
         <v>5</v>
       </c>
+      <c r="I29" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
@@ -1310,6 +1344,9 @@
       </c>
       <c r="H30">
         <v>5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1337,6 +1374,9 @@
       <c r="H31">
         <v>5</v>
       </c>
+      <c r="I31" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
@@ -1363,6 +1403,9 @@
       <c r="H32">
         <v>5</v>
       </c>
+      <c r="I32" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
@@ -1389,6 +1432,9 @@
       <c r="H33">
         <v>5</v>
       </c>
+      <c r="I33" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
@@ -1415,6 +1461,9 @@
       <c r="H34">
         <v>5</v>
       </c>
+      <c r="I34" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
@@ -1441,6 +1490,9 @@
       <c r="H35">
         <v>5</v>
       </c>
+      <c r="I35" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
@@ -1467,6 +1519,9 @@
       <c r="H36">
         <v>5</v>
       </c>
+      <c r="I36" s="13">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
@@ -1493,6 +1548,9 @@
       <c r="H37">
         <v>5</v>
       </c>
+      <c r="I37" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
@@ -1545,6 +1603,9 @@
       <c r="H39">
         <v>5</v>
       </c>
+      <c r="I39" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
@@ -1571,6 +1632,9 @@
       <c r="H40">
         <v>5</v>
       </c>
+      <c r="I40" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
@@ -1597,6 +1661,9 @@
       <c r="H41">
         <v>5</v>
       </c>
+      <c r="I41" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
@@ -1622,6 +1689,9 @@
       </c>
       <c r="H42">
         <v>5</v>
+      </c>
+      <c r="I42" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add test cases for age and rating
</commit_message>
<xml_diff>
--- a/Unit 2/Project 1 Part 1/Test Cases.xlsx
+++ b/Unit 2/Project 1 Part 1/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandoflores/Desktop/Fall 21/CSE565/Unit 2/Project 1 Part 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261AC3EA-8BCF-4541-881B-938474D99530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526DCF75-776B-FB41-9E80-42E78040EDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1760" windowWidth="33600" windowHeight="19240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25880" windowHeight="20220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Matrix" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="45">
   <si>
     <t>Defect Description</t>
   </si>
@@ -157,10 +157,19 @@
     <t>Expected Result</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>Error</t>
   </si>
   <si>
     <t>No discount given</t>
+  </si>
+  <si>
+    <t>Username length invalid</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -199,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5E69"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -254,12 +269,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5E69"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -534,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541407C-F33E-B246-BDA0-B1FB1801AAFA}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,7 +703,10 @@
         <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -708,7 +735,13 @@
         <v>5</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -737,7 +770,10 @@
         <v>5</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -766,7 +802,13 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="14" t="s">
         <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -795,7 +837,10 @@
         <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -824,7 +869,10 @@
         <v>5</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -853,7 +901,13 @@
         <v>5</v>
       </c>
       <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="12" t="s">
         <v>40</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -882,7 +936,10 @@
         <v>5</v>
       </c>
       <c r="I14" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -911,7 +968,7 @@
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -940,7 +997,7 @@
         <v>5</v>
       </c>
       <c r="I16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -969,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="I17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -998,30 +1055,30 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19" s="9">
         <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19">
-        <v>24</v>
+      <c r="C19" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G19" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H19">
         <v>5</v>
@@ -1031,31 +1088,28 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
-        <v>24</v>
-      </c>
-      <c r="D20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20">
-        <v>5</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="A20" s="9">
+        <v>14</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="11">
+        <v>5</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1076,7 +1130,7 @@
         <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G21" t="s">
         <v>36</v>
@@ -1085,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1105,7 +1159,7 @@
         <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G22" t="s">
         <v>17</v>
@@ -1113,8 +1167,8 @@
       <c r="H22">
         <v>5</v>
       </c>
-      <c r="I22" s="13">
-        <v>0.1</v>
+      <c r="I22" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1134,7 +1188,7 @@
         <v>32</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
         <v>36</v>
@@ -1143,7 +1197,7 @@
         <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1163,7 +1217,7 @@
         <v>32</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
         <v>17</v>
@@ -1171,8 +1225,8 @@
       <c r="H24">
         <v>5</v>
       </c>
-      <c r="I24" t="s">
-        <v>41</v>
+      <c r="I24" s="13">
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1192,7 +1246,7 @@
         <v>32</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s">
         <v>36</v>
@@ -1201,7 +1255,7 @@
         <v>5</v>
       </c>
       <c r="I25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1221,7 +1275,7 @@
         <v>32</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G26" t="s">
         <v>17</v>
@@ -1230,7 +1284,7 @@
         <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1247,10 +1301,10 @@
         <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G27" t="s">
         <v>36</v>
@@ -1259,11 +1313,11 @@
         <v>5</v>
       </c>
       <c r="I27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="5">
+      <c r="A28" s="1">
         <v>22</v>
       </c>
       <c r="B28" t="s">
@@ -1276,39 +1330,39 @@
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
         <v>34</v>
-      </c>
-      <c r="G28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28">
-        <v>5</v>
-      </c>
-      <c r="I28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="5">
-        <v>23</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29">
-        <v>24</v>
-      </c>
-      <c r="D29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" t="s">
-        <v>16</v>
       </c>
       <c r="G29" t="s">
         <v>36</v>
@@ -1317,11 +1371,11 @@
         <v>5</v>
       </c>
       <c r="I29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="5">
+      <c r="A30" s="1">
         <v>24</v>
       </c>
       <c r="B30" t="s">
@@ -1337,36 +1391,36 @@
         <v>15</v>
       </c>
       <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>24</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
         <v>16</v>
-      </c>
-      <c r="G30" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30">
-        <v>5</v>
-      </c>
-      <c r="I30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
-        <v>25</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31">
-        <v>24</v>
-      </c>
-      <c r="D31" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" t="s">
-        <v>35</v>
       </c>
       <c r="G31" t="s">
         <v>36</v>
@@ -1375,11 +1429,11 @@
         <v>5</v>
       </c>
       <c r="I31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
+      <c r="A32" s="1">
         <v>26</v>
       </c>
       <c r="B32" t="s">
@@ -1395,36 +1449,36 @@
         <v>15</v>
       </c>
       <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
         <v>35</v>
-      </c>
-      <c r="G32" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32">
-        <v>5</v>
-      </c>
-      <c r="I32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
-        <v>27</v>
-      </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33">
-        <v>24</v>
-      </c>
-      <c r="D33" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" t="s">
-        <v>37</v>
       </c>
       <c r="G33" t="s">
         <v>36</v>
@@ -1433,11 +1487,11 @@
         <v>5</v>
       </c>
       <c r="I33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
+      <c r="A34" s="1">
         <v>28</v>
       </c>
       <c r="B34" t="s">
@@ -1453,78 +1507,78 @@
         <v>15</v>
       </c>
       <c r="F34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="I34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
         <v>37</v>
       </c>
-      <c r="G34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34">
-        <v>5</v>
-      </c>
-      <c r="I34" s="13">
+      <c r="G35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+      <c r="I36" s="13">
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
-        <v>29</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35">
-        <v>24</v>
-      </c>
-      <c r="D35" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H35">
-        <v>5</v>
-      </c>
-      <c r="I35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
-        <v>30</v>
-      </c>
-      <c r="B36" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36">
-        <v>24</v>
-      </c>
-      <c r="D36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36">
-        <v>5</v>
-      </c>
-      <c r="I36" s="13">
-        <v>0.25</v>
-      </c>
-    </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
+      <c r="A37" s="1">
         <v>31</v>
       </c>
       <c r="B37" t="s">
@@ -1540,7 +1594,7 @@
         <v>33</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>36</v>
@@ -1549,11 +1603,11 @@
         <v>5</v>
       </c>
       <c r="I37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+      <c r="A38" s="1">
         <v>32</v>
       </c>
       <c r="B38" t="s">
@@ -1569,7 +1623,7 @@
         <v>33</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>17</v>
@@ -1577,9 +1631,12 @@
       <c r="H38">
         <v>5</v>
       </c>
+      <c r="I38" s="13">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+      <c r="A39" s="1">
         <v>33</v>
       </c>
       <c r="B39" t="s">
@@ -1595,7 +1652,7 @@
         <v>33</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>36</v>
@@ -1604,11 +1661,11 @@
         <v>5</v>
       </c>
       <c r="I39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+      <c r="A40" s="1">
         <v>34</v>
       </c>
       <c r="B40" t="s">
@@ -1624,7 +1681,7 @@
         <v>33</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>17</v>
@@ -1632,12 +1689,9 @@
       <c r="H40">
         <v>5</v>
       </c>
-      <c r="I40" s="13">
-        <v>0.15</v>
-      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
+      <c r="A41" s="1">
         <v>35</v>
       </c>
       <c r="B41" t="s">
@@ -1653,7 +1707,7 @@
         <v>33</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G41" s="11" t="s">
         <v>36</v>
@@ -1662,11 +1716,11 @@
         <v>5</v>
       </c>
       <c r="I41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
+      <c r="A42" s="1">
         <v>36</v>
       </c>
       <c r="B42" t="s">
@@ -1682,49 +1736,49 @@
         <v>33</v>
       </c>
       <c r="F42" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+      <c r="I42" s="13">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>37</v>
       </c>
-      <c r="G42" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H42">
-        <v>5</v>
-      </c>
-      <c r="I42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43">
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B43" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43">
-        <v>24</v>
-      </c>
-      <c r="D43" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" t="s">
-        <v>34</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="G43" s="11" t="s">
         <v>36</v>
       </c>
       <c r="H43">
         <v>5</v>
       </c>
       <c r="I43" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="5">
+      <c r="A44" s="1">
         <v>38</v>
       </c>
       <c r="B44" t="s">
@@ -1734,26 +1788,26 @@
         <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
-      </c>
-      <c r="F44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G44" s="11" t="s">
         <v>17</v>
       </c>
       <c r="H44">
         <v>5</v>
       </c>
       <c r="I44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="5">
+      <c r="A45" s="1">
         <v>39</v>
       </c>
       <c r="B45" t="s">
@@ -1769,7 +1823,7 @@
         <v>32</v>
       </c>
       <c r="F45" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G45" t="s">
         <v>36</v>
@@ -1778,11 +1832,11 @@
         <v>5</v>
       </c>
       <c r="I45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
+      <c r="A46" s="1">
         <v>40</v>
       </c>
       <c r="B46" t="s">
@@ -1798,7 +1852,7 @@
         <v>32</v>
       </c>
       <c r="F46" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G46" t="s">
         <v>17</v>
@@ -1807,11 +1861,11 @@
         <v>5</v>
       </c>
       <c r="I46" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="5">
+      <c r="A47" s="1">
         <v>41</v>
       </c>
       <c r="B47" t="s">
@@ -1827,7 +1881,7 @@
         <v>32</v>
       </c>
       <c r="F47" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G47" t="s">
         <v>36</v>
@@ -1836,11 +1890,11 @@
         <v>5</v>
       </c>
       <c r="I47" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="5">
+      <c r="A48" s="1">
         <v>42</v>
       </c>
       <c r="B48" t="s">
@@ -1856,7 +1910,7 @@
         <v>32</v>
       </c>
       <c r="F48" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G48" t="s">
         <v>17</v>
@@ -1865,11 +1919,11 @@
         <v>5</v>
       </c>
       <c r="I48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="5">
+      <c r="A49" s="1">
         <v>43</v>
       </c>
       <c r="B49" t="s">
@@ -1885,7 +1939,7 @@
         <v>32</v>
       </c>
       <c r="F49" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G49" t="s">
         <v>36</v>
@@ -1894,11 +1948,11 @@
         <v>5</v>
       </c>
       <c r="I49" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="5">
+      <c r="A50" s="1">
         <v>44</v>
       </c>
       <c r="B50" t="s">
@@ -1914,7 +1968,7 @@
         <v>32</v>
       </c>
       <c r="F50" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G50" t="s">
         <v>17</v>
@@ -1923,11 +1977,11 @@
         <v>5</v>
       </c>
       <c r="I50" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="5">
+      <c r="A51" s="1">
         <v>45</v>
       </c>
       <c r="B51" t="s">
@@ -1940,10 +1994,10 @@
         <v>30</v>
       </c>
       <c r="E51" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F51" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G51" t="s">
         <v>36</v>
@@ -1952,11 +2006,11 @@
         <v>5</v>
       </c>
       <c r="I51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="5">
+      <c r="A52" s="1">
         <v>46</v>
       </c>
       <c r="B52" t="s">
@@ -1969,10 +2023,10 @@
         <v>30</v>
       </c>
       <c r="E52" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F52" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G52" t="s">
         <v>17</v>
@@ -1981,11 +2035,11 @@
         <v>5</v>
       </c>
       <c r="I52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="5">
+      <c r="A53" s="1">
         <v>47</v>
       </c>
       <c r="B53" t="s">
@@ -2001,7 +2055,7 @@
         <v>15</v>
       </c>
       <c r="F53" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G53" t="s">
         <v>36</v>
@@ -2010,11 +2064,11 @@
         <v>5</v>
       </c>
       <c r="I53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="5">
+      <c r="A54" s="1">
         <v>48</v>
       </c>
       <c r="B54" t="s">
@@ -2030,7 +2084,7 @@
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G54" t="s">
         <v>17</v>
@@ -2039,11 +2093,11 @@
         <v>5</v>
       </c>
       <c r="I54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="5">
+      <c r="A55" s="1">
         <v>49</v>
       </c>
       <c r="B55" t="s">
@@ -2059,7 +2113,7 @@
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G55" t="s">
         <v>36</v>
@@ -2068,11 +2122,11 @@
         <v>5</v>
       </c>
       <c r="I55" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="5">
+      <c r="A56" s="1">
         <v>50</v>
       </c>
       <c r="B56" t="s">
@@ -2088,7 +2142,7 @@
         <v>15</v>
       </c>
       <c r="F56" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G56" t="s">
         <v>17</v>
@@ -2097,11 +2151,11 @@
         <v>5</v>
       </c>
       <c r="I56" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="5">
+      <c r="A57" s="1">
         <v>51</v>
       </c>
       <c r="B57" t="s">
@@ -2117,7 +2171,7 @@
         <v>15</v>
       </c>
       <c r="F57" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G57" t="s">
         <v>36</v>
@@ -2126,11 +2180,11 @@
         <v>5</v>
       </c>
       <c r="I57" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="5">
+      <c r="A58" s="1">
         <v>52</v>
       </c>
       <c r="B58" t="s">
@@ -2146,7 +2200,7 @@
         <v>15</v>
       </c>
       <c r="F58" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G58" t="s">
         <v>17</v>
@@ -2155,11 +2209,11 @@
         <v>5</v>
       </c>
       <c r="I58" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="5">
+      <c r="A59" s="1">
         <v>53</v>
       </c>
       <c r="B59" t="s">
@@ -2172,23 +2226,23 @@
         <v>30</v>
       </c>
       <c r="E59" t="s">
-        <v>33</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G59" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" t="s">
+        <v>37</v>
+      </c>
+      <c r="G59" t="s">
         <v>36</v>
       </c>
       <c r="H59">
         <v>5</v>
       </c>
       <c r="I59" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="5">
+      <c r="A60" s="1">
         <v>54</v>
       </c>
       <c r="B60" t="s">
@@ -2201,23 +2255,23 @@
         <v>30</v>
       </c>
       <c r="E60" t="s">
-        <v>33</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G60" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" t="s">
+        <v>37</v>
+      </c>
+      <c r="G60" t="s">
         <v>17</v>
       </c>
       <c r="H60">
         <v>5</v>
       </c>
       <c r="I60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="5">
+      <c r="A61" s="1">
         <v>55</v>
       </c>
       <c r="B61" t="s">
@@ -2233,7 +2287,7 @@
         <v>33</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G61" s="11" t="s">
         <v>36</v>
@@ -2242,11 +2296,11 @@
         <v>5</v>
       </c>
       <c r="I61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="5">
+      <c r="A62" s="1">
         <v>56</v>
       </c>
       <c r="B62" t="s">
@@ -2262,7 +2316,7 @@
         <v>33</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G62" s="11" t="s">
         <v>17</v>
@@ -2271,11 +2325,11 @@
         <v>5</v>
       </c>
       <c r="I62" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="5">
+      <c r="A63" s="1">
         <v>57</v>
       </c>
       <c r="B63" t="s">
@@ -2291,7 +2345,7 @@
         <v>33</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G63" s="11" t="s">
         <v>36</v>
@@ -2300,11 +2354,11 @@
         <v>5</v>
       </c>
       <c r="I63" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="5">
+      <c r="A64" s="1">
         <v>58</v>
       </c>
       <c r="B64" t="s">
@@ -2320,7 +2374,7 @@
         <v>33</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G64" s="11" t="s">
         <v>17</v>
@@ -2329,11 +2383,11 @@
         <v>5</v>
       </c>
       <c r="I64" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="5">
+      <c r="A65" s="1">
         <v>59</v>
       </c>
       <c r="B65" t="s">
@@ -2349,7 +2403,7 @@
         <v>33</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G65" s="11" t="s">
         <v>36</v>
@@ -2358,11 +2412,11 @@
         <v>5</v>
       </c>
       <c r="I65" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="5">
+      <c r="A66" s="1">
         <v>60</v>
       </c>
       <c r="B66" t="s">
@@ -2378,81 +2432,81 @@
         <v>33</v>
       </c>
       <c r="F66" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>61</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67">
+        <v>24</v>
+      </c>
+      <c r="D67" t="s">
+        <v>30</v>
+      </c>
+      <c r="E67" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G66" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H66">
-        <v>5</v>
-      </c>
-      <c r="I66" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="5">
-        <v>61</v>
-      </c>
-      <c r="B67" t="s">
-        <v>21</v>
-      </c>
-      <c r="C67" s="12">
-        <v>24</v>
-      </c>
-      <c r="D67" t="s">
-        <v>14</v>
-      </c>
-      <c r="E67" t="s">
-        <v>15</v>
-      </c>
-      <c r="F67" t="s">
-        <v>38</v>
-      </c>
-      <c r="G67" t="s">
-        <v>17</v>
+      <c r="G67" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="H67">
-        <v>1</v>
-      </c>
-      <c r="I67" s="11" t="s">
-        <v>41</v>
+        <v>5</v>
+      </c>
+      <c r="I67" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="5">
+      <c r="A68" s="1">
         <v>62</v>
       </c>
       <c r="B68" t="s">
         <v>21</v>
       </c>
-      <c r="C68" s="12">
+      <c r="C68">
         <v>24</v>
       </c>
       <c r="D68" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E68" t="s">
-        <v>15</v>
-      </c>
-      <c r="F68" t="s">
-        <v>38</v>
-      </c>
-      <c r="G68" t="s">
+        <v>33</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G68" s="11" t="s">
         <v>17</v>
       </c>
       <c r="H68">
-        <v>10</v>
-      </c>
-      <c r="I68" s="11" t="s">
-        <v>41</v>
+        <v>5</v>
+      </c>
+      <c r="I68" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="9">
+      <c r="A69" s="1">
         <v>63</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B69" t="s">
         <v>21</v>
       </c>
       <c r="C69" s="12">
@@ -2470,18 +2524,18 @@
       <c r="G69" t="s">
         <v>17</v>
       </c>
-      <c r="H69" s="2">
-        <v>0</v>
-      </c>
-      <c r="I69" t="s">
-        <v>40</v>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="9">
+      <c r="A70" s="1">
         <v>64</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B70" t="s">
         <v>21</v>
       </c>
       <c r="C70" s="12">
@@ -2499,27 +2553,133 @@
       <c r="G70" t="s">
         <v>17</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H70">
+        <v>10</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="9">
+        <v>65</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" s="12">
+        <v>24</v>
+      </c>
+      <c r="D71" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" t="s">
+        <v>38</v>
+      </c>
+      <c r="G71" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0</v>
+      </c>
+      <c r="I71" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="9">
+        <v>66</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C72" s="12">
+        <v>24</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>15</v>
+      </c>
+      <c r="F72" t="s">
+        <v>38</v>
+      </c>
+      <c r="G72" t="s">
+        <v>17</v>
+      </c>
+      <c r="H72" s="2">
         <v>11</v>
       </c>
-      <c r="I70" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
+      <c r="I72" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
+      <c r="A73" s="9">
+        <v>67</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" s="12">
+        <v>24</v>
+      </c>
+      <c r="D73" t="s">
+        <v>14</v>
+      </c>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" t="s">
+        <v>38</v>
+      </c>
+      <c r="G73" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I73" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="9">
+        <v>68</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" s="12">
+        <v>24</v>
+      </c>
+      <c r="D74" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" t="s">
+        <v>38</v>
+      </c>
+      <c r="G74" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I74" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>